<commit_message>
Add sending leter task
</commit_message>
<xml_diff>
--- a/DataSource/excel/task.xlsx
+++ b/DataSource/excel/task.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujiel/Dropbox (Personal)/Code/gitCode/SalingGame/DataSource/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="task.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -160,48 +165,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t>利润的形式
-0： 固定利润
-1：百分比利润</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -270,7 +239,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>_</t>
@@ -311,18 +279,6 @@
     <t>startCity</t>
   </si>
   <si>
-    <t>profitType</t>
-  </si>
-  <si>
-    <t>profitValue</t>
-  </si>
-  <si>
-    <t>depositType</t>
-  </si>
-  <si>
-    <t>depositValue</t>
-  </si>
-  <si>
     <t>taskTitleId</t>
   </si>
   <si>
@@ -345,7 +301,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -802,13 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -819,11 +774,9 @@
     <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -831,10 +784,10 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -846,28 +799,16 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -898,20 +839,8 @@
       <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -940,22 +869,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -984,22 +901,10 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>50</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1028,22 +933,10 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>50</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1072,22 +965,10 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1095,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -1116,22 +997,10 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>50</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>50</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1139,7 +1008,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -1160,22 +1029,10 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1206,20 +1063,8 @@
       <c r="J9">
         <v>10</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>50</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1250,20 +1095,8 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>50</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1294,20 +1127,8 @@
       <c r="J11">
         <v>10</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>50</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1338,20 +1159,8 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>50</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1382,20 +1191,8 @@
       <c r="J13">
         <v>5</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>50</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1426,20 +1223,8 @@
       <c r="J14">
         <v>5</v>
       </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>50</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1470,20 +1255,8 @@
       <c r="J15">
         <v>5</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>50</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1513,28 +1286,11 @@
       </c>
       <c r="J16">
         <v>0</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>50</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>